<commit_message>
core update before discussion with team
</commit_message>
<xml_diff>
--- a/Data/ADZ_2017Dec_combined04_attributes.xlsx
+++ b/Data/ADZ_2017Dec_combined04_attributes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kim Haw Lee\LEEKH\DSGA\QGIS Online Courses\QGIS Vanguard slide deck\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Projects\qgis-vanguard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1DF9DD6-772D-46D7-9CAC-9686962EA1BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEBE120-0301-4D7D-80A0-03768BB279A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6D651685-051F-4244-B982-D601680A7A12}"/>
+    <workbookView xWindow="3852" yWindow="744" windowWidth="17820" windowHeight="10512" xr2:uid="{6D651685-051F-4244-B982-D601680A7A12}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes_definition" sheetId="2" r:id="rId1"/>
@@ -21,20 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="179">
   <si>
     <t>Attribute</t>
   </si>
@@ -42,12 +34,6 @@
     <t>Definition</t>
   </si>
   <si>
-    <t>ADZ_ID</t>
-  </si>
-  <si>
-    <t>ADZ ID</t>
-  </si>
-  <si>
     <t>BET0TO2</t>
   </si>
   <si>
@@ -117,24 +103,6 @@
     <t>OVER85</t>
   </si>
   <si>
-    <t>TOTALRES</t>
-  </si>
-  <si>
-    <t>total residents</t>
-  </si>
-  <si>
-    <t>MALES</t>
-  </si>
-  <si>
-    <t>total male residents</t>
-  </si>
-  <si>
-    <t>FEMALES</t>
-  </si>
-  <si>
-    <t>total female residents</t>
-  </si>
-  <si>
     <t>Avg_AV_E</t>
   </si>
   <si>
@@ -411,24 +379,9 @@
     <t>Total count of junior college (JC) or centralised institute (CI) students</t>
   </si>
   <si>
-    <t>Active_</t>
-  </si>
-  <si>
-    <t>Active CPF member counts</t>
-  </si>
-  <si>
-    <t>Others_</t>
-  </si>
-  <si>
     <t>Inactive or self-employed CPF member counts</t>
   </si>
   <si>
-    <t>Total_CPF</t>
-  </si>
-  <si>
-    <t>Total CPF member counts</t>
-  </si>
-  <si>
     <t>w_500_blw_</t>
   </si>
   <si>
@@ -513,12 +466,6 @@
     <t>CPF member industry: Manufacturing</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>CPF member industry: Electricity,Gas&amp;Air-Con Supply</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -609,22 +556,13 @@
     <t>CPF member industry: Other Service Activities</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>CPF member industry: EmployersOfDomesticPersonnel</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>CPF member industry: Extra-TerritorialOrganisations</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>CPF member industry: Not Adequately Defined</t>
+    <t>VariableX</t>
+  </si>
+  <si>
+    <t>An unknown independent Variable</t>
+  </si>
+  <si>
+    <t>Ina_CPF_N</t>
   </si>
 </sst>
 </file>
@@ -699,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -710,6 +648,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1026,11 +967,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A336F810-DD81-4E6B-9388-AC1EC2DEA0CB}">
-  <dimension ref="A1:B109"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1061,179 +1002,179 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -1241,7 +1182,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -1249,7 +1190,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -1273,7 +1214,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -1281,7 +1222,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -1289,7 +1230,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -1297,7 +1238,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B33" s="4" t="s">
@@ -1594,322 +1535,250 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B99" s="4" t="s">
+      <c r="A99" s="6" t="s">
         <v>176</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B101" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B102" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="B105" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="B108" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="B109" s="4" t="s">
-        <v>196</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>